<commit_message>
update aftern prod deployment
</commit_message>
<xml_diff>
--- a/release-tracking/release-tracking.xlsx
+++ b/release-tracking/release-tracking.xlsx
@@ -194,8 +194,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -220,13 +222,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -559,7 +563,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -606,6 +610,9 @@
       </c>
       <c r="C2" s="4">
         <v>43207.645833333336</v>
+      </c>
+      <c r="D2" s="4">
+        <v>43208.645833333336</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>16</v>

</xml_diff>